<commit_message>
Rerunning plots and creating latex table.
</commit_message>
<xml_diff>
--- a/code/results/storm_j10_7200/benders_results_j10.xlsx
+++ b/code/results/storm_j10_7200/benders_results_j10.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2264" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2273" uniqueCount="563">
   <si>
     <t xml:space="preserve">instance</t>
   </si>
@@ -1642,6 +1642,12 @@
     <t xml:space="preserve">j1064_2</t>
   </si>
   <si>
+    <t xml:space="preserve">percent solved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">average percent solved</t>
+  </si>
+  <si>
     <t xml:space="preserve">j1064_3</t>
   </si>
   <si>
@@ -1655,6 +1661,9 @@
   </si>
   <si>
     <t xml:space="preserve">(excl. instances where no feasible solution was found)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">average avg. gap</t>
   </si>
   <si>
     <t xml:space="preserve">j1064_5</t>
@@ -1678,10 +1687,16 @@
     <t xml:space="preserve">median iterations</t>
   </si>
   <si>
+    <t xml:space="preserve">average median iterations</t>
+  </si>
+  <si>
     <t xml:space="preserve">j1064_8</t>
   </si>
   <si>
     <t xml:space="preserve">avg. iteration time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">average avg iteration time</t>
   </si>
   <si>
     <t xml:space="preserve">j1064_9</t>
@@ -1706,11 +1721,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1726,12 +1742,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1776,16 +1786,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1806,10 +1812,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L537"/>
+  <dimension ref="A1:Q537"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A508" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M546" activeCellId="0" sqref="M546"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I508" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R539" activeCellId="0" sqref="R539"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15578,10 +15584,24 @@
       <c r="H529" s="0" t="n">
         <v>0.961</v>
       </c>
+      <c r="J529" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="K529" s="0" t="n">
+        <f aca="false">100*COUNTIF(E2:E537,0)/ROWS(E2:E537)</f>
+        <v>99.6268656716418</v>
+      </c>
+      <c r="P529" s="0" t="s">
+        <v>540</v>
+      </c>
+      <c r="Q529" s="0" t="n">
+        <f aca="false">AVERAGE(benders_results_0:benders_results_7!K529:K529)</f>
+        <v>79.8041044776119</v>
+      </c>
     </row>
     <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A530" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="B530" s="0" t="n">
         <v>0</v>
@@ -15605,7 +15625,7 @@
         <v>0.891</v>
       </c>
       <c r="J530" s="1" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="K530" s="1" t="n">
         <f aca="false">COUNTIF(E2:E537,0)</f>
@@ -15615,7 +15635,7 @@
     </row>
     <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="0" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="B531" s="0" t="n">
         <v>0</v>
@@ -15639,19 +15659,26 @@
         <v>0.574</v>
       </c>
       <c r="J531" s="1" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="K531" s="1" t="n">
         <f aca="false">AVERAGEIF(E2:E537,"&lt;&gt;*nan")</f>
         <v>0</v>
       </c>
       <c r="L531" s="1" t="s">
-        <v>543</v>
+        <v>545</v>
+      </c>
+      <c r="P531" s="0" t="s">
+        <v>546</v>
+      </c>
+      <c r="Q531" s="0" t="n">
+        <f aca="false">AVERAGE(benders_results_0:benders_results_7!K531:K531)</f>
+        <v>0.0462865168539326</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="0" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="B532" s="0" t="n">
         <v>0</v>
@@ -15675,19 +15702,19 @@
         <v>1.45</v>
       </c>
       <c r="J532" s="1" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="K532" s="1" t="e">
         <f aca="false">AVERAGEIFS(E2:E537,E2:E537,"&lt;&gt;*nan",E2:E537,"&lt;&gt;0")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L532" s="2" t="s">
-        <v>543</v>
+      <c r="L532" s="1" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="0" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="B533" s="0" t="n">
         <v>0</v>
@@ -15711,19 +15738,19 @@
         <v>0.508</v>
       </c>
       <c r="J533" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="K533" s="1" t="n">
         <f aca="false">AVERAGEIF(F2:F537,"&lt;&gt;0")</f>
         <v>1</v>
       </c>
       <c r="L533" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="0" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="B534" s="0" t="n">
         <v>0</v>
@@ -15747,19 +15774,26 @@
         <v>0.854</v>
       </c>
       <c r="J534" s="1" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="K534" s="1" t="n">
         <f aca="false">MEDIAN(IF(F2:F537&lt;&gt;0,F2:F537))</f>
         <v>1</v>
       </c>
       <c r="L534" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
+      </c>
+      <c r="P534" s="0" t="s">
+        <v>554</v>
+      </c>
+      <c r="Q534" s="0" t="n">
+        <f aca="false">AVERAGE(benders_results_0:benders_results_7!K534:K534)</f>
+        <v>39.375</v>
       </c>
     </row>
     <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A535" s="0" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="B535" s="0" t="n">
         <v>0</v>
@@ -15783,19 +15817,26 @@
         <v>0.593</v>
       </c>
       <c r="J535" s="1" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
       <c r="K535" s="1" t="n">
         <f aca="false">AVERAGEIF(G2:G537,"&lt;&gt;*inf")</f>
         <v>73.5987958801497</v>
       </c>
       <c r="L535" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
+      </c>
+      <c r="P535" s="0" t="s">
+        <v>557</v>
+      </c>
+      <c r="Q535" s="0" t="n">
+        <f aca="false">AVERAGE(benders_results_0:benders_results_7!K535:K535)</f>
+        <v>68.4096741573033</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="0" t="s">
-        <v>553</v>
+        <v>558</v>
       </c>
       <c r="B536" s="0" t="n">
         <v>0</v>
@@ -15819,19 +15860,26 @@
         <v>0.86</v>
       </c>
       <c r="J536" s="1" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
       <c r="K536" s="1" t="n">
         <f aca="false">AVERAGE(H2:H537)</f>
         <v>100.380322761194</v>
       </c>
       <c r="L536" s="1" t="s">
-        <v>555</v>
+        <v>560</v>
+      </c>
+      <c r="P536" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="Q536" s="0" t="n">
+        <f aca="false">AVERAGE(benders_results_0:benders_results_7!K536:K536)</f>
+        <v>1669.71024580224</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="0" t="s">
-        <v>556</v>
+        <v>561</v>
       </c>
       <c r="B537" s="0" t="n">
         <v>0</v>
@@ -15855,7 +15903,7 @@
         <v>0.901</v>
       </c>
       <c r="J537" s="1" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
       <c r="K537" s="1" t="n">
         <f aca="false">AVERAGEIF(H2:H537,"&lt;7200")</f>
@@ -15882,7 +15930,7 @@
   <dimension ref="A1:L537"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A508" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J530" activeCellId="0" sqref="J530"/>
+      <selection pane="topLeft" activeCell="Q529" activeCellId="0" sqref="Q529"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29651,10 +29699,17 @@
       <c r="H529" s="0" t="n">
         <v>21.933</v>
       </c>
+      <c r="J529" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="K529" s="0" t="n">
+        <f aca="false">100*COUNTIF(E2:E537,0)/ROWS(E2:E537)</f>
+        <v>75</v>
+      </c>
     </row>
     <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A530" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="B530" s="0" t="n">
         <v>3</v>
@@ -29678,7 +29733,7 @@
         <v>36.551</v>
       </c>
       <c r="J530" s="1" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="K530" s="1" t="n">
         <f aca="false">COUNTIF(E2:E537,0)</f>
@@ -29688,7 +29743,7 @@
     </row>
     <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="0" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="B531" s="0" t="n">
         <v>3</v>
@@ -29712,19 +29767,19 @@
         <v>3.359</v>
       </c>
       <c r="J531" s="1" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="K531" s="1" t="n">
         <f aca="false">AVERAGEIF(E2:E537,"&lt;&gt;*nan")</f>
         <v>0.0523089887640449</v>
       </c>
       <c r="L531" s="1" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="0" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="B532" s="0" t="n">
         <v>3</v>
@@ -29748,19 +29803,19 @@
         <v>85.989</v>
       </c>
       <c r="J532" s="1" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="K532" s="1" t="n">
         <f aca="false">AVERAGEIFS(E2:E537,E2:E537,"&lt;&gt;*nan",E2:E537,"&lt;&gt;0")</f>
         <v>0.211613636363636</v>
       </c>
-      <c r="L532" s="2" t="s">
-        <v>543</v>
+      <c r="L532" s="1" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="0" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="B533" s="0" t="n">
         <v>3</v>
@@ -29784,19 +29839,19 @@
         <v>16.328</v>
       </c>
       <c r="J533" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="K533" s="1" t="n">
         <f aca="false">AVERAGEIF(F2:F537,"&lt;&gt;0")</f>
         <v>78.4119850187266</v>
       </c>
       <c r="L533" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="0" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="B534" s="0" t="n">
         <v>3</v>
@@ -29820,19 +29875,19 @@
         <v>17.941</v>
       </c>
       <c r="J534" s="1" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="K534" s="1" t="n">
         <f aca="false">MEDIAN(IF(F2:F537&lt;&gt;0,F2:F537))</f>
         <v>48.5</v>
       </c>
       <c r="L534" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A535" s="0" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="B535" s="0" t="n">
         <v>3</v>
@@ -29856,19 +29911,19 @@
         <v>8.623</v>
       </c>
       <c r="J535" s="1" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
       <c r="K535" s="1" t="n">
         <f aca="false">AVERAGEIF(G2:G537,"&lt;&gt;*inf")</f>
         <v>64.0654269662921</v>
       </c>
       <c r="L535" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="0" t="s">
-        <v>553</v>
+        <v>558</v>
       </c>
       <c r="B536" s="0" t="n">
         <v>3</v>
@@ -29892,19 +29947,19 @@
         <v>16.686</v>
       </c>
       <c r="J536" s="1" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
       <c r="K536" s="1" t="n">
         <f aca="false">AVERAGE(H2:H537)</f>
         <v>2065.58897014925</v>
       </c>
       <c r="L536" s="1" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="0" t="s">
-        <v>556</v>
+        <v>561</v>
       </c>
       <c r="B537" s="0" t="n">
         <v>3</v>
@@ -29928,7 +29983,7 @@
         <v>45.614</v>
       </c>
       <c r="J537" s="1" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
       <c r="K537" s="1" t="n">
         <f aca="false">AVERAGEIF(H2:H537,"&lt;7200")</f>
@@ -29939,7 +29994,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -29955,7 +30010,7 @@
   <dimension ref="A1:L537"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A507" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J530" activeCellId="0" sqref="J530"/>
+      <selection pane="topLeft" activeCell="G549" activeCellId="0" sqref="G549"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -43724,10 +43779,17 @@
       <c r="H529" s="0" t="n">
         <v>26.469</v>
       </c>
+      <c r="J529" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="K529" s="0" t="n">
+        <f aca="false">100*COUNTIF(E2:E537,0)/ROWS(E2:E537)</f>
+        <v>72.7611940298507</v>
+      </c>
     </row>
     <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A530" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="B530" s="0" t="n">
         <v>5</v>
@@ -43751,7 +43813,7 @@
         <v>39.954</v>
       </c>
       <c r="J530" s="1" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="K530" s="1" t="n">
         <f aca="false">COUNTIF(E2:E537,0)</f>
@@ -43761,7 +43823,7 @@
     </row>
     <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="0" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="B531" s="0" t="n">
         <v>5</v>
@@ -43785,19 +43847,19 @@
         <v>2.994</v>
       </c>
       <c r="J531" s="1" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="K531" s="1" t="n">
         <f aca="false">AVERAGEIF(E2:E537,"&lt;&gt;*nan")</f>
         <v>0.0653220973782772</v>
       </c>
       <c r="L531" s="1" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="0" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="B532" s="0" t="n">
         <v>5</v>
@@ -43821,19 +43883,19 @@
         <v>89.681</v>
       </c>
       <c r="J532" s="1" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="K532" s="1" t="n">
         <f aca="false">AVERAGEIFS(E2:E537,E2:E537,"&lt;&gt;*nan",E2:E537,"&lt;&gt;0")</f>
         <v>0.242236111111111</v>
       </c>
-      <c r="L532" s="2" t="s">
-        <v>543</v>
+      <c r="L532" s="1" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="0" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="B533" s="0" t="n">
         <v>5</v>
@@ -43857,19 +43919,19 @@
         <v>14.269</v>
       </c>
       <c r="J533" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="K533" s="1" t="n">
         <f aca="false">AVERAGEIF(F2:F537,"&lt;&gt;0")</f>
         <v>86.0767790262172</v>
       </c>
       <c r="L533" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="0" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="B534" s="0" t="n">
         <v>5</v>
@@ -43893,19 +43955,19 @@
         <v>17.584</v>
       </c>
       <c r="J534" s="1" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="K534" s="1" t="n">
         <f aca="false">MEDIAN(IF(F2:F537&lt;&gt;0,F2:F537))</f>
         <v>53.5</v>
       </c>
       <c r="L534" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A535" s="0" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="B535" s="0" t="n">
         <v>5</v>
@@ -43929,19 +43991,19 @@
         <v>8.288</v>
       </c>
       <c r="J535" s="1" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
       <c r="K535" s="1" t="n">
         <f aca="false">AVERAGEIF(G2:G537,"&lt;&gt;*inf")</f>
         <v>67.8852846441947</v>
       </c>
       <c r="L535" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="0" t="s">
-        <v>553</v>
+        <v>558</v>
       </c>
       <c r="B536" s="0" t="n">
         <v>5</v>
@@ -43965,19 +44027,19 @@
         <v>17.074</v>
       </c>
       <c r="J536" s="1" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
       <c r="K536" s="1" t="n">
         <f aca="false">AVERAGE(H2:H537)</f>
         <v>2234.4799869403</v>
       </c>
       <c r="L536" s="1" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="0" t="s">
-        <v>556</v>
+        <v>561</v>
       </c>
       <c r="B537" s="0" t="n">
         <v>5</v>
@@ -44001,7 +44063,7 @@
         <v>47.432</v>
       </c>
       <c r="J537" s="1" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
       <c r="K537" s="1" t="n">
         <f aca="false">AVERAGEIF(H2:H537,"&lt;7200")</f>
@@ -44012,7 +44074,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -44028,7 +44090,7 @@
   <dimension ref="A1:L537"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A503" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J530" activeCellId="0" sqref="J530"/>
+      <selection pane="topLeft" activeCell="J529" activeCellId="0" sqref="J529"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -57797,10 +57859,17 @@
       <c r="H529" s="0" t="n">
         <v>27.461</v>
       </c>
+      <c r="J529" s="0" t="s">
+        <v>539</v>
+      </c>
+      <c r="K529" s="0" t="n">
+        <f aca="false">100*COUNTIF(E2:E537,0)/ROWS(E2:E537)</f>
+        <v>71.8283582089552</v>
+      </c>
     </row>
     <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A530" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="B530" s="0" t="n">
         <v>7</v>
@@ -57824,7 +57893,7 @@
         <v>42.352</v>
       </c>
       <c r="J530" s="1" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="K530" s="1" t="n">
         <f aca="false">COUNTIF(E2:E537,0)</f>
@@ -57834,7 +57903,7 @@
     </row>
     <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="0" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="B531" s="0" t="n">
         <v>7</v>
@@ -57858,19 +57927,19 @@
         <v>3.235</v>
       </c>
       <c r="J531" s="1" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="K531" s="1" t="n">
         <f aca="false">AVERAGEIF(E2:E537,"&lt;&gt;*nan")</f>
         <v>0.0675149812734082</v>
       </c>
       <c r="L531" s="1" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="0" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="B532" s="0" t="n">
         <v>7</v>
@@ -57894,19 +57963,19 @@
         <v>86.216</v>
       </c>
       <c r="J532" s="1" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="K532" s="1" t="n">
         <f aca="false">AVERAGEIFS(E2:E537,E2:E537,"&lt;&gt;*nan",E2:E537,"&lt;&gt;0")</f>
         <v>0.24196644295302</v>
       </c>
-      <c r="L532" s="2" t="s">
-        <v>543</v>
+      <c r="L532" s="1" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="0" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="B533" s="0" t="n">
         <v>7</v>
@@ -57930,19 +57999,19 @@
         <v>16.008</v>
       </c>
       <c r="J533" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="K533" s="1" t="n">
         <f aca="false">AVERAGEIF(F2:F537,"&lt;&gt;0")</f>
         <v>88.1760299625468</v>
       </c>
       <c r="L533" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="0" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="B534" s="0" t="n">
         <v>7</v>
@@ -57966,19 +58035,19 @@
         <v>17.613</v>
       </c>
       <c r="J534" s="1" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="K534" s="1" t="n">
         <f aca="false">MEDIAN(IF(F2:F537&lt;&gt;0,F2:F537))</f>
         <v>54.5</v>
       </c>
       <c r="L534" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A535" s="0" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="B535" s="0" t="n">
         <v>7</v>
@@ -58002,19 +58071,19 @@
         <v>9.456</v>
       </c>
       <c r="J535" s="1" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
       <c r="K535" s="1" t="n">
         <f aca="false">AVERAGEIF(G2:G537,"&lt;&gt;*inf")</f>
         <v>68.0891891385769</v>
       </c>
       <c r="L535" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="0" t="s">
-        <v>553</v>
+        <v>558</v>
       </c>
       <c r="B536" s="0" t="n">
         <v>7</v>
@@ -58038,19 +58107,19 @@
         <v>16.037</v>
       </c>
       <c r="J536" s="1" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
       <c r="K536" s="1" t="n">
         <f aca="false">AVERAGE(H2:H537)</f>
         <v>2278.39170335821</v>
       </c>
       <c r="L536" s="1" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="0" t="s">
-        <v>556</v>
+        <v>561</v>
       </c>
       <c r="B537" s="0" t="n">
         <v>7</v>
@@ -58074,7 +58143,7 @@
         <v>46.026</v>
       </c>
       <c r="J537" s="1" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
       <c r="K537" s="1" t="n">
         <f aca="false">AVERAGEIF(H2:H537,"&lt;7200")</f>
@@ -58085,7 +58154,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>